<commit_message>
low wage offers for reference person introduced into model
</commit_message>
<xml_diff>
--- a/input/reg_socialcare.xlsx
+++ b/input/reg_socialcare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88695655-2479-49A3-B118-BD522AF67ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534F022D-089D-43BA-AC2B-221F415B5823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="551" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="551" firstSheet="14" activeTab="21" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -884,9 +884,6 @@
     <t>S3e</t>
   </si>
   <si>
-    <t>Probit regression estimates for the incidence of informal care to non-partners where person is providing care to a partner</t>
-  </si>
-  <si>
     <t>care for partner (lag, Ref = no care)</t>
   </si>
   <si>
@@ -908,9 +905,6 @@
     <t>Notes: Sample limited to individuals aged 18 and over with partners to whom they provide informal care and without missing variables. Weighted estimates with robust standard errors. "lag" defined as preceding year. Regional dummy variables generally not significant, and omitted from table for brevity (available from authors upon request).</t>
   </si>
   <si>
-    <t>Probit regression estimates for the incidence of informal care to non-partners where person is not providing care to a partner</t>
-  </si>
-  <si>
     <t>Care for partner (lag, Ref = no care)</t>
   </si>
   <si>
@@ -924,9 +918,6 @@
   </si>
   <si>
     <t>distinguishes between no care provision and only provision to non-partner - used when projecting population through time</t>
-  </si>
-  <si>
-    <t>Probit regression estimates for the incidence of informal care for people who do not have a partner</t>
   </si>
   <si>
     <t>distinguishes between no care provision and only provision to non-partner - used when evaluating expectations for behaviour</t>
@@ -1326,6 +1317,15 @@
   </si>
   <si>
     <t>Model parameters governing projection of demand for social care and supply of informal care</t>
+  </si>
+  <si>
+    <t>Probit regression estimates for the incidence of informal care provision to non-partners where person is providing care to a partner</t>
+  </si>
+  <si>
+    <t>Probit regression estimates for the incidence of informal care provision to non-partners where person is not providing care to a partner</t>
+  </si>
+  <si>
+    <t>Probit regression estimates for the incidence of informal care provision for people who do not have a partner</t>
   </si>
 </sst>
 </file>
@@ -1940,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F25AC8-F3A4-45E4-B3D4-29D900575D65}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,7 +1956,7 @@
         <v>113</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
         <v>115</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
       </c>
       <c r="B19" s="9" t="str">
         <f>'Process 3a'!A1</f>
-        <v>Probit regression estimates for the incidence of informal care to non-partners where person is providing care to a partner</v>
+        <v>Probit regression estimates for the incidence of informal care provision to non-partners where person is providing care to a partner</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B20" s="9" t="str">
         <f>'Process 3b'!A1</f>
-        <v>Probit regression estimates for the incidence of informal care to non-partners where person is not providing care to a partner</v>
+        <v>Probit regression estimates for the incidence of informal care provision to non-partners where person is not providing care to a partner</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="B21" s="9" t="str">
         <f>'Process S3c'!A1</f>
-        <v>Probit regression estimates for the incidence of informal care for people who do not have a partner</v>
+        <v>Probit regression estimates for the incidence of informal care provision for people who do not have a partner</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -9064,13 +9064,13 @@
         <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="K1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="L1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="M1" t="s">
         <v>251</v>
@@ -9941,7 +9941,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B9">
         <v>-0.13468015449712439</v>
@@ -10054,7 +10054,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B10">
         <v>1.2360594696402825</v>
@@ -10167,7 +10167,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B11">
         <v>1.2526743455656943</v>
@@ -13151,13 +13151,13 @@
         <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="K1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="L1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="M1" t="s">
         <v>136</v>
@@ -13202,7 +13202,7 @@
         <v>263</v>
       </c>
       <c r="AA1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AB1" t="s">
         <v>28</v>
@@ -14076,7 +14076,7 @@
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B9">
         <v>0.25869233445896295</v>
@@ -14195,7 +14195,7 @@
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B10">
         <v>1.5142504338202676</v>
@@ -14314,7 +14314,7 @@
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B11">
         <v>1.8060831570926916</v>
@@ -17688,13 +17688,13 @@
         <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="K1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="L1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="M1" t="s">
         <v>251</v>
@@ -17736,7 +17736,7 @@
         <v>263</v>
       </c>
       <c r="Z1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="AA1" t="s">
         <v>28</v>
@@ -18589,7 +18589,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B9">
         <v>0.39977195757379846</v>
@@ -18705,7 +18705,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B10">
         <v>1.1982019384889886</v>
@@ -18821,7 +18821,7 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B11">
         <v>1.7782700768396966</v>
@@ -21974,243 +21974,243 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" t="s">
+        <v>300</v>
+      </c>
+      <c r="F1" t="s">
         <v>301</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>302</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>303</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>304</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>373</v>
+      </c>
+      <c r="K1" t="s">
+        <v>376</v>
+      </c>
+      <c r="L1" t="s">
+        <v>370</v>
+      </c>
+      <c r="M1" t="s">
         <v>305</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>306</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1" t="s">
         <v>307</v>
       </c>
-      <c r="J1" t="s">
-        <v>376</v>
-      </c>
-      <c r="K1" t="s">
-        <v>379</v>
-      </c>
-      <c r="L1" t="s">
-        <v>373</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>308</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>309</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>310</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>311</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>312</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>313</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>314</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>315</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>316</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>317</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>318</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>319</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>320</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>348</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>350</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>377</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>352</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>355</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>356</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>357</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>358</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>364</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>365</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>366</v>
+      </c>
+      <c r="BC1" t="s">
         <v>321</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="BD1" t="s">
         <v>322</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="BE1" t="s">
         <v>323</v>
       </c>
-      <c r="AC1" t="s">
-        <v>347</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>348</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>349</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>350</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>351</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>352</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>353</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>377</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>380</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>374</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>354</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>355</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>356</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>357</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>358</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>359</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>360</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>361</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>363</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>364</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>365</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>366</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>367</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>368</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>369</v>
-      </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>324</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>325</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>326</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>327</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
+        <v>375</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>378</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>372</v>
+      </c>
+      <c r="BM1" t="s">
         <v>328</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BN1" t="s">
         <v>329</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BO1" t="s">
         <v>330</v>
       </c>
-      <c r="BJ1" t="s">
-        <v>378</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>381</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>375</v>
-      </c>
-      <c r="BM1" t="s">
+      <c r="BP1" t="s">
         <v>331</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BQ1" t="s">
         <v>332</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BR1" t="s">
         <v>333</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
         <v>334</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BT1" t="s">
         <v>335</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BU1" t="s">
         <v>336</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BV1" t="s">
         <v>337</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BW1" t="s">
         <v>338</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BX1" t="s">
         <v>339</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BY1" t="s">
         <v>340</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BZ1" t="s">
         <v>341</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="CA1" t="s">
         <v>342</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="CB1" t="s">
         <v>343</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>344</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>345</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B2">
         <v>-2.7616936035943316E-2</v>
@@ -22452,7 +22452,7 @@
     </row>
     <row r="3" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B3">
         <v>0.36572065914342194</v>
@@ -22694,7 +22694,7 @@
     </row>
     <row r="4" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B4">
         <v>0.63249987889921022</v>
@@ -22936,7 +22936,7 @@
     </row>
     <row r="5" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B5">
         <v>4.5050375271087191E-2</v>
@@ -23178,7 +23178,7 @@
     </row>
     <row r="6" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B6">
         <v>0.19127315884644083</v>
@@ -23420,7 +23420,7 @@
     </row>
     <row r="7" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B7">
         <v>0.52237795163905199</v>
@@ -23662,7 +23662,7 @@
     </row>
     <row r="8" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B8">
         <v>0.60648409798777547</v>
@@ -23904,7 +23904,7 @@
     </row>
     <row r="9" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B9">
         <v>4.7066360608284494</v>
@@ -24146,7 +24146,7 @@
     </row>
     <row r="10" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B10">
         <v>4.5486352195460649</v>
@@ -24388,7 +24388,7 @@
     </row>
     <row r="11" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B11">
         <v>0.40359882407003134</v>
@@ -24630,7 +24630,7 @@
     </row>
     <row r="12" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B12">
         <v>6.9353846669294644E-2</v>
@@ -24872,7 +24872,7 @@
     </row>
     <row r="13" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B13">
         <v>0.25054488755056825</v>
@@ -25114,7 +25114,7 @@
     </row>
     <row r="14" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B14">
         <v>0.65086612397210797</v>
@@ -25356,7 +25356,7 @@
     </row>
     <row r="15" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B15">
         <v>1.2029721772231932</v>
@@ -25598,7 +25598,7 @@
     </row>
     <row r="16" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B16">
         <v>9.4063102729240983E-2</v>
@@ -25840,7 +25840,7 @@
     </row>
     <row r="17" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B17">
         <v>5.1828069397896019E-2</v>
@@ -26082,7 +26082,7 @@
     </row>
     <row r="18" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B18">
         <v>-4.3892655459313028E-2</v>
@@ -26324,7 +26324,7 @@
     </row>
     <row r="19" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B19">
         <v>-0.10932274568152381</v>
@@ -26566,7 +26566,7 @@
     </row>
     <row r="20" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B20">
         <v>5.0318700087640784E-2</v>
@@ -26808,7 +26808,7 @@
     </row>
     <row r="21" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B21">
         <v>-0.1958766561888905</v>
@@ -27050,7 +27050,7 @@
     </row>
     <row r="22" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B22">
         <v>-0.15028726206222104</v>
@@ -27292,7 +27292,7 @@
     </row>
     <row r="23" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B23">
         <v>-2.075337886545384E-2</v>
@@ -27534,7 +27534,7 @@
     </row>
     <row r="24" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B24">
         <v>-6.1394087335860971E-2</v>
@@ -27776,7 +27776,7 @@
     </row>
     <row r="25" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B25">
         <v>1.9097163456355717E-2</v>
@@ -28018,7 +28018,7 @@
     </row>
     <row r="26" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B26">
         <v>2.3156367556155012E-2</v>
@@ -28260,7 +28260,7 @@
     </row>
     <row r="27" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B27">
         <v>-5.0683019630344219</v>
@@ -28502,7 +28502,7 @@
     </row>
     <row r="28" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B28">
         <v>-0.19427060041754729</v>
@@ -28744,7 +28744,7 @@
     </row>
     <row r="29" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B29">
         <v>0.41033740945659852</v>
@@ -28986,7 +28986,7 @@
     </row>
     <row r="30" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B30">
         <v>0.41509811723840584</v>
@@ -29228,7 +29228,7 @@
     </row>
     <row r="31" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B31">
         <v>9.4035667733039882E-2</v>
@@ -29470,7 +29470,7 @@
     </row>
     <row r="32" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B32">
         <v>0.21808131413650544</v>
@@ -29712,7 +29712,7 @@
     </row>
     <row r="33" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B33">
         <v>0.61063844466657813</v>
@@ -29954,7 +29954,7 @@
     </row>
     <row r="34" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B34">
         <v>0.72216771794884582</v>
@@ -30196,7 +30196,7 @@
     </row>
     <row r="35" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B35">
         <v>4.6005819611151235</v>
@@ -30438,7 +30438,7 @@
     </row>
     <row r="36" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B36">
         <v>6.7710410126570704</v>
@@ -30680,7 +30680,7 @@
     </row>
     <row r="37" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B37">
         <v>2.5612786702436328</v>
@@ -30922,7 +30922,7 @@
     </row>
     <row r="38" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B38">
         <v>0.29158463003193269</v>
@@ -31164,7 +31164,7 @@
     </row>
     <row r="39" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B39">
         <v>0.5723585772773</v>
@@ -31406,7 +31406,7 @@
     </row>
     <row r="40" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B40">
         <v>0.55389710257385616</v>
@@ -31648,7 +31648,7 @@
     </row>
     <row r="41" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B41">
         <v>0.47248412475356</v>
@@ -31890,7 +31890,7 @@
     </row>
     <row r="42" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B42">
         <v>0.20046270789397441</v>
@@ -32132,7 +32132,7 @@
     </row>
     <row r="43" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B43">
         <v>-5.982223562122968E-2</v>
@@ -32374,7 +32374,7 @@
     </row>
     <row r="44" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="B44">
         <v>2.788450425966656E-2</v>
@@ -32616,7 +32616,7 @@
     </row>
     <row r="45" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B45">
         <v>-0.2024158744828643</v>
@@ -32858,7 +32858,7 @@
     </row>
     <row r="46" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B46">
         <v>8.976515647364712E-2</v>
@@ -33100,7 +33100,7 @@
     </row>
     <row r="47" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B47">
         <v>-0.22431341765199117</v>
@@ -33342,7 +33342,7 @@
     </row>
     <row r="48" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B48">
         <v>-9.071014613384254E-2</v>
@@ -33584,7 +33584,7 @@
     </row>
     <row r="49" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B49">
         <v>-0.20165909911584196</v>
@@ -33826,7 +33826,7 @@
     </row>
     <row r="50" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B50">
         <v>5.2161914649696883E-2</v>
@@ -34068,7 +34068,7 @@
     </row>
     <row r="51" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B51">
         <v>-0.12347447645867128</v>
@@ -34310,7 +34310,7 @@
     </row>
     <row r="52" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B52">
         <v>0.26340465623408549</v>
@@ -34552,7 +34552,7 @@
     </row>
     <row r="53" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B53">
         <v>-6.6225720056532262</v>
@@ -34794,7 +34794,7 @@
     </row>
     <row r="54" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B54">
         <v>-0.33644637713360609</v>
@@ -35036,7 +35036,7 @@
     </row>
     <row r="55" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B55">
         <v>0.15706283607648713</v>
@@ -35278,7 +35278,7 @@
     </row>
     <row r="56" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B56">
         <v>-5.8575600742218438E-2</v>
@@ -35520,7 +35520,7 @@
     </row>
     <row r="57" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B57">
         <v>0.15454424673129313</v>
@@ -35762,7 +35762,7 @@
     </row>
     <row r="58" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B58">
         <v>0.15692009996394987</v>
@@ -36004,7 +36004,7 @@
     </row>
     <row r="59" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B59">
         <v>0.14018074080866927</v>
@@ -36246,7 +36246,7 @@
     </row>
     <row r="60" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B60">
         <v>-2.5751444609815557E-2</v>
@@ -36488,7 +36488,7 @@
     </row>
     <row r="61" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B61">
         <v>0.31668775133088661</v>
@@ -36730,7 +36730,7 @@
     </row>
     <row r="62" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B62">
         <v>2.7420880310071145</v>
@@ -36972,7 +36972,7 @@
     </row>
     <row r="63" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B63">
         <v>3.1975522647774861</v>
@@ -37214,7 +37214,7 @@
     </row>
     <row r="64" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B64">
         <v>0.29580631817527459</v>
@@ -37456,7 +37456,7 @@
     </row>
     <row r="65" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B65">
         <v>0.62620538085393518</v>
@@ -37698,7 +37698,7 @@
     </row>
     <row r="66" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B66">
         <v>0.70125323720227739</v>
@@ -37940,7 +37940,7 @@
     </row>
     <row r="67" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B67">
         <v>0.19889900775965319</v>
@@ -38182,7 +38182,7 @@
     </row>
     <row r="68" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B68">
         <v>0.12540892712839397</v>
@@ -38424,7 +38424,7 @@
     </row>
     <row r="69" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B69">
         <v>-2.3529997307720506E-2</v>
@@ -38666,7 +38666,7 @@
     </row>
     <row r="70" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B70">
         <v>-4.6636374503210218E-2</v>
@@ -38908,7 +38908,7 @@
     </row>
     <row r="71" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B71">
         <v>0.13530141963088171</v>
@@ -39150,7 +39150,7 @@
     </row>
     <row r="72" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B72">
         <v>0.13170490222608633</v>
@@ -39392,7 +39392,7 @@
     </row>
     <row r="73" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B73">
         <v>4.8176817755592301E-2</v>
@@ -39634,7 +39634,7 @@
     </row>
     <row r="74" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B74">
         <v>-5.3460760277513871E-3</v>
@@ -39876,7 +39876,7 @@
     </row>
     <row r="75" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B75">
         <v>4.9216064484720545E-2</v>
@@ -40118,7 +40118,7 @@
     </row>
     <row r="76" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B76">
         <v>5.5205410832971362E-2</v>
@@ -40360,7 +40360,7 @@
     </row>
     <row r="77" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B77">
         <v>1.0680771598910515E-2</v>
@@ -40602,7 +40602,7 @@
     </row>
     <row r="78" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B78">
         <v>6.8960412749350206E-2</v>
@@ -40844,7 +40844,7 @@
     </row>
     <row r="79" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B79">
         <v>-3.2735627176095972</v>
@@ -41128,10 +41128,10 @@
         <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="L1" t="s">
         <v>136</v>
@@ -42029,7 +42029,7 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B9">
         <v>-0.20462041162760941</v>
@@ -42145,7 +42145,7 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B10">
         <v>-1.2723230033686566</v>
@@ -46383,7 +46383,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -46525,7 +46525,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
@@ -46533,7 +46533,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B15" s="8">
         <v>-0.20462040000000001</v>
@@ -46547,7 +46547,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B16" s="8">
         <v>-1.2723230000000001</v>
@@ -46851,7 +46851,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -47079,23 +47079,23 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="37" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="38"/>
       <c r="E2" s="37" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="F2" s="38"/>
       <c r="G2" s="38"/>
       <c r="H2" s="37" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I2" s="38"/>
       <c r="J2" s="38"/>
@@ -47250,7 +47250,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="42"/>
       <c r="C9" s="8"/>
@@ -47264,7 +47264,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10" s="42">
         <v>4.7066359999999996</v>
@@ -47296,7 +47296,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" s="42">
         <v>4.548635</v>
@@ -47328,7 +47328,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" s="42">
         <v>0.40359879999999998</v>
@@ -47502,7 +47502,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="8"/>
@@ -47516,7 +47516,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B19" s="42">
         <v>6.9353799999999993E-2</v>
@@ -47548,7 +47548,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B20" s="42">
         <v>0.25054490000000001</v>
@@ -47580,7 +47580,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B21" s="42">
         <v>0.6508661</v>
@@ -47612,7 +47612,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B22" s="42">
         <v>1.2029719999999999</v>
@@ -47680,17 +47680,17 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -48054,9 +48054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015EFB6B-7043-420F-ACC1-42287328EA5E}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -48065,12 +48063,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>285</v>
+        <v>418</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -48142,7 +48140,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
@@ -48150,7 +48148,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10" s="8">
         <v>0.39977200000000002</v>
@@ -48164,7 +48162,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" s="8">
         <v>1.198202</v>
@@ -48178,7 +48176,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" s="8">
         <v>1.77827</v>
@@ -48503,12 +48501,12 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -48682,9 +48680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2B4F9D-B3E8-4A90-8B93-00EF36D5DB61}">
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="K63" sqref="K63"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -48693,12 +48689,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>279</v>
+        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -48770,7 +48766,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
@@ -48778,7 +48774,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10" s="8">
         <v>0.25869229999999999</v>
@@ -48792,7 +48788,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" s="8">
         <v>1.5142500000000001</v>
@@ -48806,7 +48802,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" s="8">
         <v>1.8060830000000001</v>
@@ -49066,7 +49062,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B31" s="8">
         <v>0.10614510000000001</v>
@@ -49154,12 +49150,12 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="27" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -49386,8 +49382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9104025-97C2-445F-8B24-6FDFF8620E89}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49397,12 +49393,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>271</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -49480,7 +49476,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
@@ -49488,7 +49484,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B10" s="8">
         <v>-0.1346802</v>
@@ -49505,7 +49501,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B11" s="8">
         <v>1.236059</v>
@@ -49519,7 +49515,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B12" s="8">
         <v>1.2526740000000001</v>
@@ -49762,7 +49758,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B30" s="8">
         <v>0.16388259999999999</v>
@@ -49797,7 +49793,7 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D32" s="8"/>
     </row>
@@ -49862,12 +49858,12 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -53051,19 +53047,19 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4" s="46" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C4" s="47"/>
       <c r="D4" s="47"/>
       <c r="E4" s="46" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F4" s="47"/>
       <c r="G4" s="47"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B5" s="48">
         <v>0.20569999999999999</v>
@@ -53160,7 +53156,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="7"/>
@@ -53171,7 +53167,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B11" s="42">
         <v>-1.24369</v>
@@ -53610,7 +53606,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B29" s="7">
         <v>0.67159999999999997</v>
@@ -53650,13 +53646,13 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="I33" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J33" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="K33" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="M33" s="3"/>
     </row>
@@ -55332,7 +55328,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B4">
         <v>0.1048</v>
@@ -55340,7 +55336,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -55371,7 +55367,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -55395,7 +55391,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="H8">
         <f>EXP(SUMPRODUCT(E6:E10,B6:B10))</f>
@@ -55408,7 +55404,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B9" s="8">
         <v>1.086568</v>
@@ -55423,7 +55419,7 @@
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="H9">
         <f>EXP(SUMPRODUCT(E6:E10,B14:B18))</f>
@@ -55451,7 +55447,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H10">
         <f>EXP(SUMPRODUCT(E6:E10,B22:B26))</f>
@@ -55472,7 +55468,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B12" s="7">
         <v>4.0599999999999997E-2</v>
@@ -55480,7 +55476,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -55527,7 +55523,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B17" s="8">
         <v>1.4185779999999999</v>
@@ -55560,7 +55556,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B20" s="7">
         <v>2.3800000000000002E-2</v>
@@ -55568,7 +55564,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -55615,7 +55611,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B25" s="8">
         <v>16.037739999999999</v>
@@ -55651,7 +55647,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B28">
         <v>0.83089999999999997</v>
@@ -55670,12 +55666,12 @@
     <row r="30" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="27" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -55735,7 +55731,7 @@
       <c r="F3" s="47"/>
       <c r="G3" s="47"/>
       <c r="M3" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="N3">
         <v>-2.279099511458512</v>
@@ -55848,7 +55844,7 @@
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B4" s="48">
         <v>8.2199999999999995E-2</v>
@@ -55974,7 +55970,7 @@
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B5" s="41"/>
       <c r="E5" s="41"/>
@@ -56092,7 +56088,7 @@
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B6" s="42">
         <v>-2.2791000000000001</v>
@@ -56649,7 +56645,7 @@
         <v>0.42099999999999999</v>
       </c>
       <c r="M10" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="N10">
         <v>-1.7005020955485395</v>
@@ -57154,7 +57150,7 @@
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B14" s="49">
         <v>0.16400000000000001</v>
@@ -57280,7 +57276,7 @@
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B15" s="41"/>
       <c r="E15" s="41"/>
@@ -57398,7 +57394,7 @@
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B16" s="42">
         <v>-4.2610349999999997</v>
@@ -57553,7 +57549,7 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="M17" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N17">
         <v>-4.2610353839923469</v>
@@ -58455,7 +58451,7 @@
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B24" s="48">
         <v>0.2492</v>
@@ -58463,7 +58459,7 @@
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
       <c r="M24" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="N24">
         <v>-2.6283666776981001</v>
@@ -58576,7 +58572,7 @@
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B25" s="41"/>
       <c r="M25" t="s">
@@ -58693,7 +58689,7 @@
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B26" s="42">
         <v>-4.1452429999999998</v>
@@ -59330,7 +59326,7 @@
         <v>0</v>
       </c>
       <c r="M31" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="N31">
         <v>-4.1452426545231829</v>
@@ -59690,7 +59686,7 @@
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B34">
         <v>0.3609</v>
@@ -61364,7 +61360,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K31" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -62520,7 +62516,7 @@
         <v>9.3399999999999997E-2</v>
       </c>
       <c r="J29" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -63064,7 +63060,7 @@
         <v>8.3056985079833119</v>
       </c>
       <c r="K28" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -69603,7 +69599,7 @@
         <v>140</v>
       </c>
       <c r="F1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G1" t="s">
         <v>177</v>
@@ -69660,7 +69656,7 @@
         <v>156</v>
       </c>
       <c r="Y1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="Z1" t="s">
         <v>179</v>
@@ -70076,7 +70072,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B5">
         <v>-1.2436896081034186</v>
@@ -72394,7 +72390,7 @@
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B24">
         <v>-2.5431662925720966</v>
@@ -75346,7 +75342,7 @@
         <v>185</v>
       </c>
       <c r="F1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G1" t="s">
         <v>170</v>
@@ -75361,7 +75357,7 @@
         <v>188</v>
       </c>
       <c r="K1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="L1" t="s">
         <v>171</v>
@@ -75376,7 +75372,7 @@
         <v>191</v>
       </c>
       <c r="P1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Q1" t="s">
         <v>172</v>
@@ -75543,7 +75539,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B5">
         <v>1.0865680091838372</v>
@@ -75808,7 +75804,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B10">
         <v>1.4185779996704873</v>
@@ -76073,7 +76069,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B15">
         <v>16.03774458448558</v>
@@ -76203,7 +76199,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D1" t="s">
         <v>192</v>
@@ -76224,7 +76220,7 @@
         <v>173</v>
       </c>
       <c r="J1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="K1" t="s">
         <v>197</v>
@@ -76245,7 +76241,7 @@
         <v>174</v>
       </c>
       <c r="Q1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="R1" t="s">
         <v>207</v>
@@ -76266,7 +76262,7 @@
         <v>212</v>
       </c>
       <c r="X1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="Y1" t="s">
         <v>202</v>
@@ -76287,7 +76283,7 @@
         <v>219</v>
       </c>
       <c r="AE1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="AF1" t="s">
         <v>213</v>
@@ -76310,7 +76306,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B2">
         <v>-2.279099511458512</v>
@@ -77101,7 +77097,7 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B9">
         <v>-1.7005020955485395</v>
@@ -77892,7 +77888,7 @@
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B16">
         <v>-4.2610353839923469</v>
@@ -78683,7 +78679,7 @@
     </row>
     <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B23">
         <v>-2.6283666776981001</v>
@@ -79474,7 +79470,7 @@
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B30">
         <v>-4.1452426545231829</v>

</xml_diff>

<commit_message>
update model parameters other than wages and income
</commit_message>
<xml_diff>
--- a/input/reg_socialcare.xlsx
+++ b/input/reg_socialcare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534F022D-089D-43BA-AC2B-221F415B5823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7629F9-73DB-4BC8-A96C-E640C503A17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="551" firstSheet="14" activeTab="21" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="551" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="421">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -1327,6 +1327,12 @@
   <si>
     <t>Probit regression estimates for the incidence of informal care provision for people who do not have a partner</t>
   </si>
+  <si>
+    <t>Authors:</t>
+  </si>
+  <si>
+    <t>Justin van de Ven</t>
+  </si>
 </sst>
 </file>
 
@@ -1938,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6F25AC8-F3A4-45E4-B3D4-29D900575D65}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,194 +1967,202 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>114</v>
+        <v>419</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>39</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B4" s="9" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-    </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B6" s="28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="9" t="str">
+      <c r="B7" s="9" t="str">
         <f>'Process 1a'!A1</f>
         <v>Probit regression describing probability of receiving informal social care: under 65</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="9" t="str">
+      <c r="B8" s="9" t="str">
         <f>'Process 1b'!A1</f>
         <v>Linear regression describing log hours of informal social care received: under 65</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="9" t="str">
+      <c r="B9" s="9" t="str">
         <f>'Process 2a'!A1</f>
         <v>Probit regression describing probability of needing assistance with ADLs: 65+</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="9" t="str">
+      <c r="B10" s="9" t="str">
         <f>'Process 2b'!A1</f>
         <v>Probit regression describing probability of receiving assistance with ADLs: 65+</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="9" t="str">
+      <c r="B11" s="9" t="str">
         <f>'Process 2c'!A1</f>
         <v>Multinomial logit regression describing split of population receiving social care, between only informal, informal and formal, and only formal markets: 65+</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B11" s="9" t="str">
+      <c r="B12" s="9" t="str">
         <f>'Process 2d'!A1</f>
         <v>Probit receive care from partner: 65+</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B12" s="9" t="str">
+      <c r="B13" s="9" t="str">
         <f>'Process 2e'!A1</f>
         <v>Mlogit for supplementary informal carers where partner provide care: 65+</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B13" s="9" t="str">
+      <c r="B14" s="9" t="str">
         <f>'Process 2f'!A1</f>
         <v>Mlogit for informal carers where partner not providing care: 65+</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="9" t="str">
+      <c r="B15" s="9" t="str">
         <f>'Process 2g'!A1</f>
         <v>Linear regression of log hours of care provided by partners to people aged 65+</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="9" t="str">
+      <c r="B16" s="9" t="str">
         <f>'Process 2h'!A1</f>
         <v>Linear regression of log hours of care provided by daughters to people aged 65+</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="9" t="str">
+      <c r="B17" s="9" t="str">
         <f>'Process 2i'!A1</f>
         <v>Linear regression of log hours of care provided by sons to people aged 65+</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B17" s="9" t="str">
+      <c r="B18" s="9" t="str">
         <f>'Process 2j'!A1</f>
         <v>Linear regression of log hours of care provided by others to people aged 65+</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B18" s="9" t="str">
+      <c r="B19" s="9" t="str">
         <f>'Process 2k'!A1</f>
         <v>Linear regression of log hours of formal care to people aged 65+</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>264</v>
       </c>
-      <c r="B19" s="9" t="str">
+      <c r="B20" s="9" t="str">
         <f>'Process 3a'!A1</f>
         <v>Probit regression estimates for the incidence of informal care provision to non-partners where person is providing care to a partner</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B20" s="9" t="str">
+      <c r="B21" s="9" t="str">
         <f>'Process 3b'!A1</f>
         <v>Probit regression estimates for the incidence of informal care provision to non-partners where person is not providing care to a partner</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B21" s="9" t="str">
+      <c r="B22" s="9" t="str">
         <f>'Process S3c'!A1</f>
         <v>Probit regression estimates for the incidence of informal care provision for people who do not have a partner</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B22" s="9" t="str">
+      <c r="B23" s="9" t="str">
         <f>'Process S3d'!A1</f>
         <v>Multinomial logit estimates for provision of social care by people with partners (reference group does not provide care)</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="B23" s="9" t="str">
+      <c r="B24" s="9" t="str">
         <f>'Process S3e'!A1</f>
         <v>Linear regression estimates of log hours informal care provided to anyone</v>
       </c>
@@ -48054,7 +48068,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{015EFB6B-7043-420F-ACC1-42287328EA5E}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>